<commit_message>
registered network with 50, 20 and 10 nodes
</commit_message>
<xml_diff>
--- a/Gephi Graphs/node_conversion.xlsx
+++ b/Gephi Graphs/node_conversion.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5901CA-18A1-449B-8A04-59B86DCC2DF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB48C6F-7091-46FB-BF69-BBCFD3FB9035}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5595" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1000" sheetId="1" r:id="rId1"/>
     <sheet name="500" sheetId="3" r:id="rId2"/>
     <sheet name="100" sheetId="2" r:id="rId3"/>
+    <sheet name="50" sheetId="4" r:id="rId4"/>
+    <sheet name="20" sheetId="5" r:id="rId5"/>
+    <sheet name="10" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5354" uniqueCount="5329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5514" uniqueCount="5481">
   <si>
     <t>rte[0].port++ &lt;--&gt; C &lt;--&gt; rte[68].port++;</t>
   </si>
@@ -16015,6 +16018,462 @@
   </si>
   <si>
     <t>&gt;15 min</t>
+  </si>
+  <si>
+    <t>Number of nodes: 50</t>
+  </si>
+  <si>
+    <t>rte[0].port++ &lt;--&gt; C &lt;--&gt; rte[2].port++;</t>
+  </si>
+  <si>
+    <t>rte[0].port++ &lt;--&gt; C &lt;--&gt; rte[15].port++;</t>
+  </si>
+  <si>
+    <t>rte[0].port++ &lt;--&gt; C &lt;--&gt; rte[18].port++;</t>
+  </si>
+  <si>
+    <t>rte[0].port++ &lt;--&gt; C &lt;--&gt; rte[28].port++;</t>
+  </si>
+  <si>
+    <t>rte[0].port++ &lt;--&gt; C &lt;--&gt; rte[31].port++;</t>
+  </si>
+  <si>
+    <t>rte[1].port++ &lt;--&gt; C &lt;--&gt; rte[12].port++;</t>
+  </si>
+  <si>
+    <t>rte[1].port++ &lt;--&gt; C &lt;--&gt; rte[22].port++;</t>
+  </si>
+  <si>
+    <t>rte[2].port++ &lt;--&gt; C &lt;--&gt; rte[6].port++;</t>
+  </si>
+  <si>
+    <t>rte[2].port++ &lt;--&gt; C &lt;--&gt; rte[15].port++;</t>
+  </si>
+  <si>
+    <t>rte[2].port++ &lt;--&gt; C &lt;--&gt; rte[23].port++;</t>
+  </si>
+  <si>
+    <t>rte[2].port++ &lt;--&gt; C &lt;--&gt; rte[31].port++;</t>
+  </si>
+  <si>
+    <t>rte[2].port++ &lt;--&gt; C &lt;--&gt; rte[41].port++;</t>
+  </si>
+  <si>
+    <t>rte[3].port++ &lt;--&gt; C &lt;--&gt; rte[14].port++;</t>
+  </si>
+  <si>
+    <t>rte[3].port++ &lt;--&gt; C &lt;--&gt; rte[17].port++;</t>
+  </si>
+  <si>
+    <t>rte[3].port++ &lt;--&gt; C &lt;--&gt; rte[26].port++;</t>
+  </si>
+  <si>
+    <t>rte[3].port++ &lt;--&gt; C &lt;--&gt; rte[36].port++;</t>
+  </si>
+  <si>
+    <t>rte[3].port++ &lt;--&gt; C &lt;--&gt; rte[46].port++;</t>
+  </si>
+  <si>
+    <t>rte[4].port++ &lt;--&gt; C &lt;--&gt; rte[32].port++;</t>
+  </si>
+  <si>
+    <t>rte[5].port++ &lt;--&gt; C &lt;--&gt; rte[38].port++;</t>
+  </si>
+  <si>
+    <t>rte[5].port++ &lt;--&gt; C &lt;--&gt; rte[39].port++;</t>
+  </si>
+  <si>
+    <t>rte[5].port++ &lt;--&gt; C &lt;--&gt; rte[41].port++;</t>
+  </si>
+  <si>
+    <t>rte[5].port++ &lt;--&gt; C &lt;--&gt; rte[48].port++;</t>
+  </si>
+  <si>
+    <t>rte[6].port++ &lt;--&gt; C &lt;--&gt; rte[9].port++;</t>
+  </si>
+  <si>
+    <t>rte[6].port++ &lt;--&gt; C &lt;--&gt; rte[42].port++;</t>
+  </si>
+  <si>
+    <t>rte[6].port++ &lt;--&gt; C &lt;--&gt; rte[43].port++;</t>
+  </si>
+  <si>
+    <t>rte[7].port++ &lt;--&gt; C &lt;--&gt; rte[42].port++;</t>
+  </si>
+  <si>
+    <t>rte[7].port++ &lt;--&gt; C &lt;--&gt; rte[49].port++;</t>
+  </si>
+  <si>
+    <t>rte[8].port++ &lt;--&gt; C &lt;--&gt; rte[21].port++;</t>
+  </si>
+  <si>
+    <t>rte[8].port++ &lt;--&gt; C &lt;--&gt; rte[27].port++;</t>
+  </si>
+  <si>
+    <t>rte[8].port++ &lt;--&gt; C &lt;--&gt; rte[40].port++;</t>
+  </si>
+  <si>
+    <t>rte[8].port++ &lt;--&gt; C &lt;--&gt; rte[43].port++;</t>
+  </si>
+  <si>
+    <t>rte[8].port++ &lt;--&gt; C &lt;--&gt; rte[48].port++;</t>
+  </si>
+  <si>
+    <t>rte[9].port++ &lt;--&gt; C &lt;--&gt; rte[10].port++;</t>
+  </si>
+  <si>
+    <t>rte[9].port++ &lt;--&gt; C &lt;--&gt; rte[18].port++;</t>
+  </si>
+  <si>
+    <t>rte[9].port++ &lt;--&gt; C &lt;--&gt; rte[36].port++;</t>
+  </si>
+  <si>
+    <t>rte[10].port++ &lt;--&gt; C &lt;--&gt; rte[13].port++;</t>
+  </si>
+  <si>
+    <t>rte[10].port++ &lt;--&gt; C &lt;--&gt; rte[22].port++;</t>
+  </si>
+  <si>
+    <t>rte[10].port++ &lt;--&gt; C &lt;--&gt; rte[29].port++;</t>
+  </si>
+  <si>
+    <t>rte[10].port++ &lt;--&gt; C &lt;--&gt; rte[31].port++;</t>
+  </si>
+  <si>
+    <t>rte[10].port++ &lt;--&gt; C &lt;--&gt; rte[36].port++;</t>
+  </si>
+  <si>
+    <t>rte[10].port++ &lt;--&gt; C &lt;--&gt; rte[41].port++;</t>
+  </si>
+  <si>
+    <t>rte[11].port++ &lt;--&gt; C &lt;--&gt; rte[19].port++;</t>
+  </si>
+  <si>
+    <t>rte[11].port++ &lt;--&gt; C &lt;--&gt; rte[22].port++;</t>
+  </si>
+  <si>
+    <t>rte[11].port++ &lt;--&gt; C &lt;--&gt; rte[26].port++;</t>
+  </si>
+  <si>
+    <t>rte[11].port++ &lt;--&gt; C &lt;--&gt; rte[27].port++;</t>
+  </si>
+  <si>
+    <t>rte[11].port++ &lt;--&gt; C &lt;--&gt; rte[47].port++;</t>
+  </si>
+  <si>
+    <t>rte[12].port++ &lt;--&gt; C &lt;--&gt; rte[17].port++;</t>
+  </si>
+  <si>
+    <t>rte[12].port++ &lt;--&gt; C &lt;--&gt; rte[30].port++;</t>
+  </si>
+  <si>
+    <t>rte[12].port++ &lt;--&gt; C &lt;--&gt; rte[34].port++;</t>
+  </si>
+  <si>
+    <t>rte[13].port++ &lt;--&gt; C &lt;--&gt; rte[19].port++;</t>
+  </si>
+  <si>
+    <t>rte[13].port++ &lt;--&gt; C &lt;--&gt; rte[24].port++;</t>
+  </si>
+  <si>
+    <t>rte[13].port++ &lt;--&gt; C &lt;--&gt; rte[28].port++;</t>
+  </si>
+  <si>
+    <t>rte[13].port++ &lt;--&gt; C &lt;--&gt; rte[29].port++;</t>
+  </si>
+  <si>
+    <t>rte[14].port++ &lt;--&gt; C &lt;--&gt; rte[16].port++;</t>
+  </si>
+  <si>
+    <t>rte[14].port++ &lt;--&gt; C &lt;--&gt; rte[24].port++;</t>
+  </si>
+  <si>
+    <t>rte[14].port++ &lt;--&gt; C &lt;--&gt; rte[32].port++;</t>
+  </si>
+  <si>
+    <t>rte[14].port++ &lt;--&gt; C &lt;--&gt; rte[49].port++;</t>
+  </si>
+  <si>
+    <t>rte[15].port++ &lt;--&gt; C &lt;--&gt; rte[23].port++;</t>
+  </si>
+  <si>
+    <t>rte[15].port++ &lt;--&gt; C &lt;--&gt; rte[27].port++;</t>
+  </si>
+  <si>
+    <t>rte[15].port++ &lt;--&gt; C &lt;--&gt; rte[34].port++;</t>
+  </si>
+  <si>
+    <t>rte[15].port++ &lt;--&gt; C &lt;--&gt; rte[36].port++;</t>
+  </si>
+  <si>
+    <t>rte[15].port++ &lt;--&gt; C &lt;--&gt; rte[39].port++;</t>
+  </si>
+  <si>
+    <t>rte[15].port++ &lt;--&gt; C &lt;--&gt; rte[42].port++;</t>
+  </si>
+  <si>
+    <t>rte[15].port++ &lt;--&gt; C &lt;--&gt; rte[49].port++;</t>
+  </si>
+  <si>
+    <t>rte[16].port++ &lt;--&gt; C &lt;--&gt; rte[20].port++;</t>
+  </si>
+  <si>
+    <t>rte[16].port++ &lt;--&gt; C &lt;--&gt; rte[32].port++;</t>
+  </si>
+  <si>
+    <t>rte[16].port++ &lt;--&gt; C &lt;--&gt; rte[37].port++;</t>
+  </si>
+  <si>
+    <t>rte[16].port++ &lt;--&gt; C &lt;--&gt; rte[45].port++;</t>
+  </si>
+  <si>
+    <t>rte[17].port++ &lt;--&gt; C &lt;--&gt; rte[18].port++;</t>
+  </si>
+  <si>
+    <t>rte[17].port++ &lt;--&gt; C &lt;--&gt; rte[31].port++;</t>
+  </si>
+  <si>
+    <t>rte[17].port++ &lt;--&gt; C &lt;--&gt; rte[40].port++;</t>
+  </si>
+  <si>
+    <t>rte[17].port++ &lt;--&gt; C &lt;--&gt; rte[46].port++;</t>
+  </si>
+  <si>
+    <t>rte[18].port++ &lt;--&gt; C &lt;--&gt; rte[27].port++;</t>
+  </si>
+  <si>
+    <t>rte[18].port++ &lt;--&gt; C &lt;--&gt; rte[36].port++;</t>
+  </si>
+  <si>
+    <t>rte[18].port++ &lt;--&gt; C &lt;--&gt; rte[38].port++;</t>
+  </si>
+  <si>
+    <t>rte[18].port++ &lt;--&gt; C &lt;--&gt; rte[41].port++;</t>
+  </si>
+  <si>
+    <t>rte[19].port++ &lt;--&gt; C &lt;--&gt; rte[26].port++;</t>
+  </si>
+  <si>
+    <t>rte[19].port++ &lt;--&gt; C &lt;--&gt; rte[29].port++;</t>
+  </si>
+  <si>
+    <t>rte[19].port++ &lt;--&gt; C &lt;--&gt; rte[38].port++;</t>
+  </si>
+  <si>
+    <t>rte[20].port++ &lt;--&gt; C &lt;--&gt; rte[38].port++;</t>
+  </si>
+  <si>
+    <t>rte[21].port++ &lt;--&gt; C &lt;--&gt; rte[23].port++;</t>
+  </si>
+  <si>
+    <t>rte[21].port++ &lt;--&gt; C &lt;--&gt; rte[33].port++;</t>
+  </si>
+  <si>
+    <t>rte[21].port++ &lt;--&gt; C &lt;--&gt; rte[41].port++;</t>
+  </si>
+  <si>
+    <t>rte[21].port++ &lt;--&gt; C &lt;--&gt; rte[44].port++;</t>
+  </si>
+  <si>
+    <t>rte[21].port++ &lt;--&gt; C &lt;--&gt; rte[49].port++;</t>
+  </si>
+  <si>
+    <t>rte[22].port++ &lt;--&gt; C &lt;--&gt; rte[49].port++;</t>
+  </si>
+  <si>
+    <t>rte[23].port++ &lt;--&gt; C &lt;--&gt; rte[28].port++;</t>
+  </si>
+  <si>
+    <t>rte[23].port++ &lt;--&gt; C &lt;--&gt; rte[39].port++;</t>
+  </si>
+  <si>
+    <t>rte[23].port++ &lt;--&gt; C &lt;--&gt; rte[40].port++;</t>
+  </si>
+  <si>
+    <t>rte[23].port++ &lt;--&gt; C &lt;--&gt; rte[43].port++;</t>
+  </si>
+  <si>
+    <t>rte[23].port++ &lt;--&gt; C &lt;--&gt; rte[49].port++;</t>
+  </si>
+  <si>
+    <t>rte[24].port++ &lt;--&gt; C &lt;--&gt; rte[28].port++;</t>
+  </si>
+  <si>
+    <t>rte[24].port++ &lt;--&gt; C &lt;--&gt; rte[31].port++;</t>
+  </si>
+  <si>
+    <t>rte[25].port++ &lt;--&gt; C &lt;--&gt; rte[26].port++;</t>
+  </si>
+  <si>
+    <t>rte[25].port++ &lt;--&gt; C &lt;--&gt; rte[31].port++;</t>
+  </si>
+  <si>
+    <t>rte[27].port++ &lt;--&gt; C &lt;--&gt; rte[42].port++;</t>
+  </si>
+  <si>
+    <t>rte[28].port++ &lt;--&gt; C &lt;--&gt; rte[35].port++;</t>
+  </si>
+  <si>
+    <t>rte[28].port++ &lt;--&gt; C &lt;--&gt; rte[43].port++;</t>
+  </si>
+  <si>
+    <t>rte[29].port++ &lt;--&gt; C &lt;--&gt; rte[32].port++;</t>
+  </si>
+  <si>
+    <t>rte[29].port++ &lt;--&gt; C &lt;--&gt; rte[47].port++;</t>
+  </si>
+  <si>
+    <t>rte[30].port++ &lt;--&gt; C &lt;--&gt; rte[32].port++;</t>
+  </si>
+  <si>
+    <t>rte[31].port++ &lt;--&gt; C &lt;--&gt; rte[36].port++;</t>
+  </si>
+  <si>
+    <t>rte[31].port++ &lt;--&gt; C &lt;--&gt; rte[40].port++;</t>
+  </si>
+  <si>
+    <t>rte[33].port++ &lt;--&gt; C &lt;--&gt; rte[42].port++;</t>
+  </si>
+  <si>
+    <t>rte[35].port++ &lt;--&gt; C &lt;--&gt; rte[46].port++;</t>
+  </si>
+  <si>
+    <t>rte[36].port++ &lt;--&gt; C &lt;--&gt; rte[49].port++;</t>
+  </si>
+  <si>
+    <t>rte[38].port++ &lt;--&gt; C &lt;--&gt; rte[45].port++;</t>
+  </si>
+  <si>
+    <t>rte[39].port++ &lt;--&gt; C &lt;--&gt; rte[42].port++;</t>
+  </si>
+  <si>
+    <t>rte[43].port++ &lt;--&gt; C &lt;--&gt; rte[46].port++;</t>
+  </si>
+  <si>
+    <t>rte[45].port++ &lt;--&gt; C &lt;--&gt; rte[46].port++;</t>
+  </si>
+  <si>
+    <t>rte[46].port++ &lt;--&gt; C &lt;--&gt; rte[47].port++;</t>
+  </si>
+  <si>
+    <t>rte[47].port++ &lt;--&gt; C &lt;--&gt; rte[49].port++;</t>
+  </si>
+  <si>
+    <t>Number of nodes: 20</t>
+  </si>
+  <si>
+    <t>rte[0].port++ &lt;--&gt; C &lt;--&gt; rte[4].port++;</t>
+  </si>
+  <si>
+    <t>rte[0].port++ &lt;--&gt; C &lt;--&gt; rte[8].port++;</t>
+  </si>
+  <si>
+    <t>rte[0].port++ &lt;--&gt; C &lt;--&gt; rte[13].port++;</t>
+  </si>
+  <si>
+    <t>rte[1].port++ &lt;--&gt; C &lt;--&gt; rte[7].port++;</t>
+  </si>
+  <si>
+    <t>rte[1].port++ &lt;--&gt; C &lt;--&gt; rte[13].port++;</t>
+  </si>
+  <si>
+    <t>rte[2].port++ &lt;--&gt; C &lt;--&gt; rte[10].port++;</t>
+  </si>
+  <si>
+    <t>rte[3].port++ &lt;--&gt; C &lt;--&gt; rte[10].port++;</t>
+  </si>
+  <si>
+    <t>rte[4].port++ &lt;--&gt; C &lt;--&gt; rte[10].port++;</t>
+  </si>
+  <si>
+    <t>rte[4].port++ &lt;--&gt; C &lt;--&gt; rte[19].port++;</t>
+  </si>
+  <si>
+    <t>rte[5].port++ &lt;--&gt; C &lt;--&gt; rte[11].port++;</t>
+  </si>
+  <si>
+    <t>rte[5].port++ &lt;--&gt; C &lt;--&gt; rte[14].port++;</t>
+  </si>
+  <si>
+    <t>rte[6].port++ &lt;--&gt; C &lt;--&gt; rte[7].port++;</t>
+  </si>
+  <si>
+    <t>rte[7].port++ &lt;--&gt; C &lt;--&gt; rte[8].port++;</t>
+  </si>
+  <si>
+    <t>rte[7].port++ &lt;--&gt; C &lt;--&gt; rte[10].port++;</t>
+  </si>
+  <si>
+    <t>rte[7].port++ &lt;--&gt; C &lt;--&gt; rte[12].port++;</t>
+  </si>
+  <si>
+    <t>rte[7].port++ &lt;--&gt; C &lt;--&gt; rte[18].port++;</t>
+  </si>
+  <si>
+    <t>rte[8].port++ &lt;--&gt; C &lt;--&gt; rte[15].port++;</t>
+  </si>
+  <si>
+    <t>rte[9].port++ &lt;--&gt; C &lt;--&gt; rte[19].port++;</t>
+  </si>
+  <si>
+    <t>rte[10].port++ &lt;--&gt; C &lt;--&gt; rte[12].port++;</t>
+  </si>
+  <si>
+    <t>rte[10].port++ &lt;--&gt; C &lt;--&gt; rte[16].port++;</t>
+  </si>
+  <si>
+    <t>rte[11].port++ &lt;--&gt; C &lt;--&gt; rte[16].port++;</t>
+  </si>
+  <si>
+    <t>rte[12].port++ &lt;--&gt; C &lt;--&gt; rte[18].port++;</t>
+  </si>
+  <si>
+    <t>rte[13].port++ &lt;--&gt; C &lt;--&gt; rte[15].port++;</t>
+  </si>
+  <si>
+    <t>rte[13].port++ &lt;--&gt; C &lt;--&gt; rte[18].port++;</t>
+  </si>
+  <si>
+    <t>rte[16].port++ &lt;--&gt; C &lt;--&gt; rte[17].port++;</t>
+  </si>
+  <si>
+    <t>Number of nodes: 10</t>
+  </si>
+  <si>
+    <t>rte[0].port++ &lt;--&gt; C &lt;--&gt; rte[3].port++;</t>
+  </si>
+  <si>
+    <t>rte[1].port++ &lt;--&gt; C &lt;--&gt; rte[2].port++;</t>
+  </si>
+  <si>
+    <t>rte[1].port++ &lt;--&gt; C &lt;--&gt; rte[4].port++;</t>
+  </si>
+  <si>
+    <t>rte[2].port++ &lt;--&gt; C &lt;--&gt; rte[4].port++;</t>
+  </si>
+  <si>
+    <t>rte[2].port++ &lt;--&gt; C &lt;--&gt; rte[8].port++;</t>
+  </si>
+  <si>
+    <t>rte[2].port++ &lt;--&gt; C &lt;--&gt; rte[9].port++;</t>
+  </si>
+  <si>
+    <t>rte[3].port++ &lt;--&gt; C &lt;--&gt; rte[5].port++;</t>
+  </si>
+  <si>
+    <t>rte[3].port++ &lt;--&gt; C &lt;--&gt; rte[8].port++;</t>
+  </si>
+  <si>
+    <t>rte[3].port++ &lt;--&gt; C &lt;--&gt; rte[9].port++;</t>
+  </si>
+  <si>
+    <t>rte[4].port++ &lt;--&gt; C &lt;--&gt; rte[5].port++;</t>
+  </si>
+  <si>
+    <t>rte[5].port++ &lt;--&gt; C &lt;--&gt; rte[6].port++;</t>
+  </si>
+  <si>
+    <t>rte[5].port++ &lt;--&gt; C &lt;--&gt; rte[7].port++;</t>
   </si>
 </sst>
 </file>
@@ -34107,8 +34566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13897C2-1AE9-48CC-9FFA-2010431CEF49}">
   <dimension ref="A1:D1546"/>
   <sheetViews>
-    <sheetView topLeftCell="A1495" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1546" sqref="A2:A1546"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41855,7 +42314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7031A8A-CCA5-4ABF-B760-6F9AC486B323}">
   <dimension ref="A1:A256"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A239" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A256"/>
     </sheetView>
   </sheetViews>
@@ -43143,5 +43602,853 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D464708-7307-43BF-8F63-01E65C3CE136}">
+  <dimension ref="A1:A119"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A119"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5335</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3554</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5340</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5341</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5343</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5344</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3563</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5345</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5347</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5348</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5350</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5351</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5353</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5354</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5355</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5356</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5357</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5358</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5359</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5360</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>5361</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5362</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5363</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>5364</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>5365</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>5366</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5367</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>5368</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>5370</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>5371</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5372</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>5373</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>5374</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>5375</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>5376</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>3609</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>5377</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>5378</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>5379</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>5380</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>5381</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>5382</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>5383</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>5384</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>5385</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>5386</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>5387</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>5388</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>5389</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>5391</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>5392</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>5393</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>5394</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>5395</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>5396</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>3627</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>5397</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>5398</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>5399</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>5401</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>5402</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>5403</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>5404</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>5405</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>5406</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>5407</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>5408</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>3643</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>5409</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>5410</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>5411</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>5412</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>5413</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>5414</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>5415</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>5416</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>5417</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>5418</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>5419</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>5420</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>5421</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>5422</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>5423</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>5424</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>5425</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>5426</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>5427</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>5428</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>5429</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>5430</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>5431</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>5432</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>5433</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>5434</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>5435</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>5436</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>5437</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>5438</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>5439</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>5440</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>5441</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497FF9B6-883A-42E7-8EAB-A070898EB4FC}">
+  <dimension ref="A1:A28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5443</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5446</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5449</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3829</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5450</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5451</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5453</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5454</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5455</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5456</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5457</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3579</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5458</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5459</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5460</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5462</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5463</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5464</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5465</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5466</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5467</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8F56A1-5A58-4EA2-B310-68F9424E6FB8}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5469</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5470</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5471</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5472</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5473</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5474</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5475</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5476</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5477</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5478</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5479</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5480</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated network of 500 nodes
</commit_message>
<xml_diff>
--- a/Gephi Graphs/node_conversion.xlsx
+++ b/Gephi Graphs/node_conversion.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FF56D0-E3A3-4EB1-95E6-0BFCB46AE641}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2583BC0-2DEB-4A84-B6F9-2DC032F6D555}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22464" yWindow="1056" windowWidth="21600" windowHeight="11388" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1000" sheetId="1" r:id="rId1"/>
@@ -34668,8 +34668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13897C2-1AE9-48CC-9FFA-2010431CEF49}">
   <dimension ref="A1:A1578"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A373" workbookViewId="0">
-      <selection activeCell="J1567" sqref="J1567"/>
+    <sheetView tabSelected="1" topLeftCell="A1552" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A1578"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>